<commit_message>
Tables to final report
</commit_message>
<xml_diff>
--- a/docs/table/table_result_juris_tcu_ndcg_10.xlsx
+++ b/docs/table/table_result_juris_tcu_ndcg_10.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,16 +571,16 @@
         <v>18.47</v>
       </c>
       <c r="F4" t="n">
-        <v>21.627</v>
+        <v>21.63</v>
       </c>
       <c r="G4" t="n">
-        <v>20.978</v>
+        <v>20.98</v>
       </c>
       <c r="H4" t="n">
-        <v>11.232</v>
+        <v>11.23</v>
       </c>
       <c r="I4" t="n">
-        <v>12.596</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="5">
@@ -588,7 +588,7 @@
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>sts_multihop</t>
+          <t>bm25</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
@@ -597,48 +597,44 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>17.445</v>
+        <v>55.16</v>
       </c>
       <c r="F5" t="n">
-        <v>20.49</v>
+        <v>55.71</v>
       </c>
       <c r="G5" t="n">
-        <v>19.071</v>
+        <v>55.24</v>
       </c>
       <c r="H5" t="n">
-        <v>10.102</v>
+        <v>51.05</v>
       </c>
       <c r="I5" t="n">
-        <v>9.757999999999999</v>
+        <v>52.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="C6" s="1" t="n"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>55.158</v>
+        <v>66.29000000000001</v>
       </c>
       <c r="F6" t="n">
-        <v>55.707</v>
+        <v>62.36</v>
       </c>
       <c r="G6" t="n">
-        <v>55.239</v>
+        <v>56.18</v>
       </c>
       <c r="H6" t="n">
-        <v>51.054</v>
+        <v>55.6</v>
       </c>
       <c r="I6" t="n">
-        <v>52.204</v>
+        <v>52.68</v>
       </c>
     </row>
     <row r="7">
@@ -647,77 +643,77 @@
       <c r="C7" s="1" t="n"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>66.292</v>
+        <v>72.95999999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>62.363</v>
+        <v>70.66</v>
       </c>
       <c r="G7" t="n">
-        <v>56.176</v>
+        <v>67.39</v>
       </c>
       <c r="H7" t="n">
-        <v>55.596</v>
+        <v>64.61</v>
       </c>
       <c r="I7" t="n">
-        <v>52.683</v>
+        <v>62.11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="n"/>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>72.95699999999999</v>
+        <v>21.48</v>
       </c>
       <c r="F8" t="n">
-        <v>70.65900000000001</v>
+        <v>25.88</v>
       </c>
       <c r="G8" t="n">
-        <v>67.387</v>
+        <v>24.51</v>
       </c>
       <c r="H8" t="n">
-        <v>64.611</v>
+        <v>17.75</v>
       </c>
       <c r="I8" t="n">
-        <v>62.107</v>
+        <v>19.26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C9" s="1" t="n"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>21.481</v>
+        <v>66.33</v>
       </c>
       <c r="F9" t="n">
-        <v>25.875</v>
+        <v>62.7</v>
       </c>
       <c r="G9" t="n">
-        <v>24.506</v>
+        <v>56.62</v>
       </c>
       <c r="H9" t="n">
-        <v>17.746</v>
+        <v>56.19</v>
       </c>
       <c r="I9" t="n">
-        <v>19.262</v>
+        <v>53.13</v>
       </c>
     </row>
     <row r="10">
@@ -726,58 +722,64 @@
       <c r="C10" s="1" t="n"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>66.32599999999999</v>
+        <v>73.52</v>
       </c>
       <c r="F10" t="n">
-        <v>62.702</v>
+        <v>71.25</v>
       </c>
       <c r="G10" t="n">
-        <v>56.618</v>
+        <v>68</v>
       </c>
       <c r="H10" t="n">
-        <v>56.187</v>
+        <v>65.22</v>
       </c>
       <c r="I10" t="n">
-        <v>53.133</v>
+        <v>62.56</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n"/>
-      <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="n"/>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>BASE</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
           <t>BASE</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>73.51600000000001</v>
+        <v>64.02</v>
       </c>
       <c r="F11" t="n">
-        <v>71.251</v>
+        <v>62.04</v>
       </c>
       <c r="G11" t="n">
-        <v>67.996</v>
+        <v>56.89</v>
       </c>
       <c r="H11" t="n">
-        <v>65.223</v>
+        <v>56.98</v>
       </c>
       <c r="I11" t="n">
-        <v>62.561</v>
+        <v>53.81</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
+      <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
@@ -790,25 +792,25 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>64.017</v>
+        <v>64.25</v>
       </c>
       <c r="F12" t="n">
-        <v>62.037</v>
+        <v>61.95</v>
       </c>
       <c r="G12" t="n">
-        <v>56.893</v>
+        <v>57.42</v>
       </c>
       <c r="H12" t="n">
-        <v>56.976</v>
+        <v>55.85</v>
       </c>
       <c r="I12" t="n">
-        <v>53.813</v>
+        <v>52.63</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
@@ -821,25 +823,25 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>64.248</v>
+        <v>64.23999999999999</v>
       </c>
       <c r="F13" t="n">
-        <v>61.948</v>
+        <v>63.57</v>
       </c>
       <c r="G13" t="n">
-        <v>57.42</v>
+        <v>59.61</v>
       </c>
       <c r="H13" t="n">
-        <v>55.848</v>
+        <v>57.12</v>
       </c>
       <c r="I13" t="n">
-        <v>52.629</v>
+        <v>54.84</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
@@ -852,25 +854,25 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>64.23699999999999</v>
+        <v>64.44</v>
       </c>
       <c r="F14" t="n">
-        <v>63.572</v>
+        <v>63.38</v>
       </c>
       <c r="G14" t="n">
-        <v>59.612</v>
+        <v>60.32</v>
       </c>
       <c r="H14" t="n">
-        <v>57.115</v>
+        <v>56.81</v>
       </c>
       <c r="I14" t="n">
-        <v>54.836</v>
+        <v>55.68</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
@@ -883,25 +885,25 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>64.43600000000001</v>
+        <v>64.43000000000001</v>
       </c>
       <c r="F15" t="n">
-        <v>63.385</v>
+        <v>64.27</v>
       </c>
       <c r="G15" t="n">
-        <v>60.316</v>
+        <v>61.06</v>
       </c>
       <c r="H15" t="n">
-        <v>56.808</v>
+        <v>58.34</v>
       </c>
       <c r="I15" t="n">
-        <v>55.681</v>
+        <v>56.43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
@@ -914,25 +916,25 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>64.431</v>
+        <v>63.61</v>
       </c>
       <c r="F16" t="n">
-        <v>64.27</v>
+        <v>64.26000000000001</v>
       </c>
       <c r="G16" t="n">
-        <v>61.062</v>
+        <v>61.11</v>
       </c>
       <c r="H16" t="n">
-        <v>58.345</v>
+        <v>58.18</v>
       </c>
       <c r="I16" t="n">
-        <v>56.427</v>
+        <v>56.22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
@@ -945,25 +947,25 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>63.607</v>
+        <v>63.49</v>
       </c>
       <c r="F17" t="n">
-        <v>64.255</v>
+        <v>63.9</v>
       </c>
       <c r="G17" t="n">
-        <v>61.111</v>
+        <v>61.67</v>
       </c>
       <c r="H17" t="n">
-        <v>58.175</v>
+        <v>58.14</v>
       </c>
       <c r="I17" t="n">
-        <v>56.224</v>
+        <v>57.65</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
@@ -976,25 +978,25 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>63.493</v>
+        <v>62.89</v>
       </c>
       <c r="F18" t="n">
-        <v>63.899</v>
+        <v>63.74</v>
       </c>
       <c r="G18" t="n">
-        <v>61.667</v>
+        <v>61.86</v>
       </c>
       <c r="H18" t="n">
-        <v>58.136</v>
+        <v>59.49</v>
       </c>
       <c r="I18" t="n">
-        <v>57.647</v>
+        <v>58.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
@@ -1007,25 +1009,25 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>62.886</v>
+        <v>62.63</v>
       </c>
       <c r="F19" t="n">
-        <v>63.738</v>
+        <v>63.57</v>
       </c>
       <c r="G19" t="n">
-        <v>61.863</v>
+        <v>61.74</v>
       </c>
       <c r="H19" t="n">
-        <v>59.493</v>
+        <v>59.71</v>
       </c>
       <c r="I19" t="n">
-        <v>58.2</v>
+        <v>58.62</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
@@ -1038,25 +1040,29 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>62.634</v>
+        <v>62.82</v>
       </c>
       <c r="F20" t="n">
-        <v>63.567</v>
+        <v>63.7</v>
       </c>
       <c r="G20" t="n">
-        <v>61.74</v>
+        <v>61.36</v>
       </c>
       <c r="H20" t="n">
-        <v>59.71</v>
+        <v>60.2</v>
       </c>
       <c r="I20" t="n">
-        <v>58.621</v>
+        <v>58.69</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n"/>
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>INDIR</t>
+        </is>
+      </c>
       <c r="B21" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
@@ -1065,58 +1071,48 @@
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>62.825</v>
+        <v>51.24</v>
       </c>
       <c r="F21" t="n">
-        <v>63.7</v>
+        <v>52.89</v>
       </c>
       <c r="G21" t="n">
-        <v>61.359</v>
+        <v>50.67</v>
       </c>
       <c r="H21" t="n">
-        <v>60.205</v>
+        <v>48.98</v>
       </c>
       <c r="I21" t="n">
-        <v>58.687</v>
+        <v>48.38</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>indir</t>
-        </is>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="A22" s="1" t="n"/>
+      <c r="B22" s="1" t="n"/>
+      <c r="C22" s="1" t="n"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>51.235</v>
+        <v>60.82</v>
       </c>
       <c r="F22" t="n">
-        <v>52.886</v>
+        <v>57.3</v>
       </c>
       <c r="G22" t="n">
-        <v>50.674</v>
+        <v>49.03</v>
       </c>
       <c r="H22" t="n">
-        <v>48.978</v>
+        <v>51.42</v>
       </c>
       <c r="I22" t="n">
-        <v>48.385</v>
+        <v>47.68</v>
       </c>
     </row>
     <row r="23">
@@ -1125,133 +1121,133 @@
       <c r="C23" s="1" t="n"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>60.82</v>
+        <v>65.04000000000001</v>
       </c>
       <c r="F23" t="n">
-        <v>57.305</v>
+        <v>64.2</v>
       </c>
       <c r="G23" t="n">
-        <v>49.032</v>
+        <v>58.96</v>
       </c>
       <c r="H23" t="n">
-        <v>51.418</v>
+        <v>59.86</v>
       </c>
       <c r="I23" t="n">
-        <v>47.685</v>
+        <v>56.3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="n"/>
-      <c r="C24" s="1" t="n"/>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>65.044</v>
+        <v>61.72</v>
       </c>
       <c r="F24" t="n">
-        <v>64.20099999999999</v>
+        <v>57.91</v>
       </c>
       <c r="G24" t="n">
-        <v>58.959</v>
+        <v>50.02</v>
       </c>
       <c r="H24" t="n">
-        <v>59.861</v>
+        <v>51.7</v>
       </c>
       <c r="I24" t="n">
-        <v>56.301</v>
+        <v>48.23</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C25" s="1" t="n"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>61.72</v>
+        <v>67.11</v>
       </c>
       <c r="F25" t="n">
-        <v>57.912</v>
+        <v>64.62</v>
       </c>
       <c r="G25" t="n">
-        <v>50.023</v>
+        <v>59.92</v>
       </c>
       <c r="H25" t="n">
-        <v>51.701</v>
+        <v>60.18</v>
       </c>
       <c r="I25" t="n">
-        <v>48.226</v>
+        <v>56.49</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="n"/>
+      <c r="B26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>67.11499999999999</v>
+        <v>50.03</v>
       </c>
       <c r="F26" t="n">
-        <v>64.61799999999999</v>
+        <v>51.82</v>
       </c>
       <c r="G26" t="n">
-        <v>59.918</v>
+        <v>48.25</v>
       </c>
       <c r="H26" t="n">
-        <v>60.184</v>
+        <v>47.37</v>
       </c>
       <c r="I26" t="n">
-        <v>56.492</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="B27" s="1" t="n"/>
+      <c r="C27" s="1" t="n"/>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>50.027</v>
+        <v>60.12</v>
       </c>
       <c r="F27" t="n">
-        <v>51.819</v>
+        <v>56.75</v>
       </c>
       <c r="G27" t="n">
-        <v>48.248</v>
+        <v>48.68</v>
       </c>
       <c r="H27" t="n">
-        <v>47.369</v>
+        <v>48.86</v>
       </c>
       <c r="I27" t="n">
-        <v>46.803</v>
+        <v>45.87</v>
       </c>
     </row>
     <row r="28">
@@ -1260,133 +1256,133 @@
       <c r="C28" s="1" t="n"/>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>60.123</v>
+        <v>64.26000000000001</v>
       </c>
       <c r="F28" t="n">
-        <v>56.749</v>
+        <v>64.36</v>
       </c>
       <c r="G28" t="n">
-        <v>48.679</v>
+        <v>58.9</v>
       </c>
       <c r="H28" t="n">
-        <v>48.858</v>
+        <v>58.97</v>
       </c>
       <c r="I28" t="n">
-        <v>45.867</v>
+        <v>55.87</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="n"/>
-      <c r="C29" s="1" t="n"/>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>64.25700000000001</v>
+        <v>60.9</v>
       </c>
       <c r="F29" t="n">
-        <v>64.355</v>
+        <v>57.41</v>
       </c>
       <c r="G29" t="n">
-        <v>58.899</v>
+        <v>49.38</v>
       </c>
       <c r="H29" t="n">
-        <v>58.974</v>
+        <v>49.71</v>
       </c>
       <c r="I29" t="n">
-        <v>55.866</v>
+        <v>46.48</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="n"/>
-      <c r="C30" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C30" s="1" t="n"/>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>60.904</v>
+        <v>65.89</v>
       </c>
       <c r="F30" t="n">
-        <v>57.411</v>
+        <v>65.23</v>
       </c>
       <c r="G30" t="n">
-        <v>49.379</v>
+        <v>60.12</v>
       </c>
       <c r="H30" t="n">
-        <v>49.709</v>
+        <v>59.66</v>
       </c>
       <c r="I30" t="n">
-        <v>46.48</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
-      <c r="B31" s="1" t="n"/>
-      <c r="C31" s="1" t="n"/>
+      <c r="B31" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>65.893</v>
+        <v>50.14</v>
       </c>
       <c r="F31" t="n">
-        <v>65.227</v>
+        <v>50.24</v>
       </c>
       <c r="G31" t="n">
-        <v>60.125</v>
+        <v>47.07</v>
       </c>
       <c r="H31" t="n">
-        <v>59.66</v>
+        <v>46.22</v>
       </c>
       <c r="I31" t="n">
-        <v>56.25</v>
+        <v>45.37</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C32" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="B32" s="1" t="n"/>
+      <c r="C32" s="1" t="n"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>50.135</v>
+        <v>59.26</v>
       </c>
       <c r="F32" t="n">
-        <v>50.238</v>
+        <v>56.27</v>
       </c>
       <c r="G32" t="n">
-        <v>47.07</v>
+        <v>47.88</v>
       </c>
       <c r="H32" t="n">
-        <v>46.217</v>
+        <v>48.26</v>
       </c>
       <c r="I32" t="n">
-        <v>45.368</v>
+        <v>46.14</v>
       </c>
     </row>
     <row r="33">
@@ -1395,133 +1391,133 @@
       <c r="C33" s="1" t="n"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>59.264</v>
+        <v>63.6</v>
       </c>
       <c r="F33" t="n">
-        <v>56.269</v>
+        <v>63.61</v>
       </c>
       <c r="G33" t="n">
-        <v>47.885</v>
+        <v>59.26</v>
       </c>
       <c r="H33" t="n">
-        <v>48.263</v>
+        <v>57.85</v>
       </c>
       <c r="I33" t="n">
-        <v>46.138</v>
+        <v>55.84</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="n"/>
-      <c r="C34" s="1" t="n"/>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>63.604</v>
+        <v>59.99</v>
       </c>
       <c r="F34" t="n">
-        <v>63.607</v>
+        <v>56.96</v>
       </c>
       <c r="G34" t="n">
-        <v>59.263</v>
+        <v>48.79</v>
       </c>
       <c r="H34" t="n">
-        <v>57.854</v>
+        <v>49.36</v>
       </c>
       <c r="I34" t="n">
-        <v>55.844</v>
+        <v>46.44</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="n"/>
-      <c r="C35" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C35" s="1" t="n"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>59.986</v>
+        <v>65.48999999999999</v>
       </c>
       <c r="F35" t="n">
-        <v>56.961</v>
+        <v>64.52</v>
       </c>
       <c r="G35" t="n">
-        <v>48.794</v>
+        <v>60.08</v>
       </c>
       <c r="H35" t="n">
-        <v>49.36</v>
+        <v>58.59</v>
       </c>
       <c r="I35" t="n">
-        <v>46.438</v>
+        <v>56.18</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
-      <c r="B36" s="1" t="n"/>
-      <c r="C36" s="1" t="n"/>
+      <c r="B36" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>65.489</v>
+        <v>48.51</v>
       </c>
       <c r="F36" t="n">
-        <v>64.51600000000001</v>
+        <v>48.66</v>
       </c>
       <c r="G36" t="n">
-        <v>60.084</v>
+        <v>45.15</v>
       </c>
       <c r="H36" t="n">
-        <v>58.586</v>
+        <v>45.13</v>
       </c>
       <c r="I36" t="n">
-        <v>56.184</v>
+        <v>44.91</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
-      <c r="B37" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C37" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="B37" s="1" t="n"/>
+      <c r="C37" s="1" t="n"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>48.506</v>
+        <v>59.31</v>
       </c>
       <c r="F37" t="n">
-        <v>48.657</v>
+        <v>54.48</v>
       </c>
       <c r="G37" t="n">
-        <v>45.149</v>
+        <v>47.72</v>
       </c>
       <c r="H37" t="n">
-        <v>45.127</v>
+        <v>47.91</v>
       </c>
       <c r="I37" t="n">
-        <v>44.911</v>
+        <v>45.47</v>
       </c>
     </row>
     <row r="38">
@@ -1530,133 +1526,133 @@
       <c r="C38" s="1" t="n"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>59.312</v>
+        <v>64.36</v>
       </c>
       <c r="F38" t="n">
-        <v>54.48</v>
+        <v>63.82</v>
       </c>
       <c r="G38" t="n">
-        <v>47.717</v>
+        <v>60.56</v>
       </c>
       <c r="H38" t="n">
-        <v>47.911</v>
+        <v>59.21</v>
       </c>
       <c r="I38" t="n">
-        <v>45.471</v>
+        <v>56.21</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="n"/>
-      <c r="C39" s="1" t="n"/>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>64.36199999999999</v>
+        <v>59.72</v>
       </c>
       <c r="F39" t="n">
-        <v>63.822</v>
+        <v>55.2</v>
       </c>
       <c r="G39" t="n">
-        <v>60.559</v>
+        <v>48.28</v>
       </c>
       <c r="H39" t="n">
-        <v>59.211</v>
+        <v>48.72</v>
       </c>
       <c r="I39" t="n">
-        <v>56.208</v>
+        <v>46.42</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="n"/>
-      <c r="C40" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C40" s="1" t="n"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>59.721</v>
+        <v>65.34999999999999</v>
       </c>
       <c r="F40" t="n">
-        <v>55.196</v>
+        <v>64.43000000000001</v>
       </c>
       <c r="G40" t="n">
-        <v>48.279</v>
+        <v>61.33</v>
       </c>
       <c r="H40" t="n">
-        <v>48.718</v>
+        <v>59.75</v>
       </c>
       <c r="I40" t="n">
-        <v>46.42</v>
+        <v>57.04</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="n"/>
-      <c r="C41" s="1" t="n"/>
+      <c r="B41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>65.348</v>
+        <v>46.57</v>
       </c>
       <c r="F41" t="n">
-        <v>64.434</v>
+        <v>46.89</v>
       </c>
       <c r="G41" t="n">
-        <v>61.326</v>
+        <v>41.94</v>
       </c>
       <c r="H41" t="n">
-        <v>59.749</v>
+        <v>42.64</v>
       </c>
       <c r="I41" t="n">
-        <v>57.043</v>
+        <v>42.68</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="B42" s="1" t="n"/>
+      <c r="C42" s="1" t="n"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>46.571</v>
+        <v>59.29</v>
       </c>
       <c r="F42" t="n">
-        <v>46.888</v>
+        <v>54.59</v>
       </c>
       <c r="G42" t="n">
-        <v>41.944</v>
+        <v>47.04</v>
       </c>
       <c r="H42" t="n">
-        <v>42.638</v>
+        <v>46.63</v>
       </c>
       <c r="I42" t="n">
-        <v>42.683</v>
+        <v>44.85</v>
       </c>
     </row>
     <row r="43">
@@ -1665,133 +1661,133 @@
       <c r="C43" s="1" t="n"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>59.292</v>
+        <v>63.78</v>
       </c>
       <c r="F43" t="n">
-        <v>54.586</v>
+        <v>62.92</v>
       </c>
       <c r="G43" t="n">
-        <v>47.037</v>
+        <v>59.91</v>
       </c>
       <c r="H43" t="n">
-        <v>46.629</v>
+        <v>58.16</v>
       </c>
       <c r="I43" t="n">
-        <v>44.852</v>
+        <v>55.89</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
       <c r="B44" s="1" t="n"/>
-      <c r="C44" s="1" t="n"/>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>63.781</v>
+        <v>59.49</v>
       </c>
       <c r="F44" t="n">
-        <v>62.921</v>
+        <v>55.04</v>
       </c>
       <c r="G44" t="n">
-        <v>59.909</v>
+        <v>47.86</v>
       </c>
       <c r="H44" t="n">
-        <v>58.16</v>
+        <v>48.02</v>
       </c>
       <c r="I44" t="n">
-        <v>55.894</v>
+        <v>45.53</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
       <c r="B45" s="1" t="n"/>
-      <c r="C45" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C45" s="1" t="n"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>59.49</v>
+        <v>64.25</v>
       </c>
       <c r="F45" t="n">
-        <v>55.039</v>
+        <v>63.84</v>
       </c>
       <c r="G45" t="n">
-        <v>47.855</v>
+        <v>60.22</v>
       </c>
       <c r="H45" t="n">
-        <v>48.024</v>
+        <v>58.76</v>
       </c>
       <c r="I45" t="n">
-        <v>45.53</v>
+        <v>56.37</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
-      <c r="B46" s="1" t="n"/>
-      <c r="C46" s="1" t="n"/>
+      <c r="B46" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>64.252</v>
+        <v>45.89</v>
       </c>
       <c r="F46" t="n">
-        <v>63.843</v>
+        <v>46.78</v>
       </c>
       <c r="G46" t="n">
-        <v>60.219</v>
+        <v>41.65</v>
       </c>
       <c r="H46" t="n">
-        <v>58.755</v>
+        <v>41.77</v>
       </c>
       <c r="I46" t="n">
-        <v>56.373</v>
+        <v>41.17</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n"/>
-      <c r="B47" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="C47" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="B47" s="1" t="n"/>
+      <c r="C47" s="1" t="n"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>45.889</v>
+        <v>59.05</v>
       </c>
       <c r="F47" t="n">
-        <v>46.784</v>
+        <v>54.45</v>
       </c>
       <c r="G47" t="n">
-        <v>41.647</v>
+        <v>47.13</v>
       </c>
       <c r="H47" t="n">
-        <v>41.77</v>
+        <v>47.19</v>
       </c>
       <c r="I47" t="n">
-        <v>41.169</v>
+        <v>45.24</v>
       </c>
     </row>
     <row r="48">
@@ -1800,133 +1796,133 @@
       <c r="C48" s="1" t="n"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E48" t="n">
+        <v>63.01</v>
+      </c>
+      <c r="F48" t="n">
+        <v>63.45</v>
+      </c>
+      <c r="G48" t="n">
+        <v>60.61</v>
+      </c>
+      <c r="H48" t="n">
         <v>59.05</v>
       </c>
-      <c r="F48" t="n">
-        <v>54.453</v>
-      </c>
-      <c r="G48" t="n">
-        <v>47.126</v>
-      </c>
-      <c r="H48" t="n">
-        <v>47.187</v>
-      </c>
       <c r="I48" t="n">
-        <v>45.235</v>
+        <v>56.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
       <c r="B49" s="1" t="n"/>
-      <c r="C49" s="1" t="n"/>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>63.006</v>
+        <v>59.83</v>
       </c>
       <c r="F49" t="n">
-        <v>63.448</v>
+        <v>54.58</v>
       </c>
       <c r="G49" t="n">
-        <v>60.613</v>
+        <v>47.63</v>
       </c>
       <c r="H49" t="n">
-        <v>59.048</v>
+        <v>47.44</v>
       </c>
       <c r="I49" t="n">
-        <v>56.603</v>
+        <v>45.79</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
       <c r="B50" s="1" t="n"/>
-      <c r="C50" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C50" s="1" t="n"/>
       <c r="D50" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>59.833</v>
+        <v>63.71</v>
       </c>
       <c r="F50" t="n">
-        <v>54.585</v>
+        <v>63.79</v>
       </c>
       <c r="G50" t="n">
-        <v>47.626</v>
+        <v>60.93</v>
       </c>
       <c r="H50" t="n">
-        <v>47.435</v>
+        <v>58.89</v>
       </c>
       <c r="I50" t="n">
-        <v>45.794</v>
+        <v>56.75</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n"/>
-      <c r="B51" s="1" t="n"/>
-      <c r="C51" s="1" t="n"/>
+      <c r="B51" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>63.709</v>
+        <v>44.45</v>
       </c>
       <c r="F51" t="n">
-        <v>63.792</v>
+        <v>45.83</v>
       </c>
       <c r="G51" t="n">
-        <v>60.933</v>
+        <v>40.42</v>
       </c>
       <c r="H51" t="n">
-        <v>58.888</v>
+        <v>40.51</v>
       </c>
       <c r="I51" t="n">
-        <v>56.748</v>
+        <v>39.83</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
-      <c r="B52" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="C52" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="B52" s="1" t="n"/>
+      <c r="C52" s="1" t="n"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>44.452</v>
+        <v>58.62</v>
       </c>
       <c r="F52" t="n">
-        <v>45.832</v>
+        <v>54.09</v>
       </c>
       <c r="G52" t="n">
-        <v>40.423</v>
+        <v>47.17</v>
       </c>
       <c r="H52" t="n">
-        <v>40.511</v>
+        <v>47.26</v>
       </c>
       <c r="I52" t="n">
-        <v>39.828</v>
+        <v>45.9</v>
       </c>
     </row>
     <row r="53">
@@ -1935,133 +1931,133 @@
       <c r="C53" s="1" t="n"/>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>58.615</v>
+        <v>62.85</v>
       </c>
       <c r="F53" t="n">
-        <v>54.09</v>
+        <v>63.8</v>
       </c>
       <c r="G53" t="n">
-        <v>47.171</v>
+        <v>61.8</v>
       </c>
       <c r="H53" t="n">
-        <v>47.26</v>
+        <v>59.5</v>
       </c>
       <c r="I53" t="n">
-        <v>45.896</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n"/>
       <c r="B54" s="1" t="n"/>
-      <c r="C54" s="1" t="n"/>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>62.854</v>
+        <v>59.62</v>
       </c>
       <c r="F54" t="n">
-        <v>63.799</v>
+        <v>54.36</v>
       </c>
       <c r="G54" t="n">
-        <v>61.798</v>
+        <v>47.67</v>
       </c>
       <c r="H54" t="n">
-        <v>59.501</v>
+        <v>47.87</v>
       </c>
       <c r="I54" t="n">
-        <v>57.595</v>
+        <v>46.14</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
       <c r="B55" s="1" t="n"/>
-      <c r="C55" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C55" s="1" t="n"/>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>59.616</v>
+        <v>63.9</v>
       </c>
       <c r="F55" t="n">
-        <v>54.364</v>
+        <v>64.14</v>
       </c>
       <c r="G55" t="n">
-        <v>47.666</v>
+        <v>62.42</v>
       </c>
       <c r="H55" t="n">
-        <v>47.866</v>
+        <v>59.68</v>
       </c>
       <c r="I55" t="n">
-        <v>46.136</v>
+        <v>57.9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n"/>
-      <c r="B56" s="1" t="n"/>
-      <c r="C56" s="1" t="n"/>
+      <c r="B56" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>63.902</v>
+        <v>44.08</v>
       </c>
       <c r="F56" t="n">
-        <v>64.13800000000001</v>
+        <v>45.64</v>
       </c>
       <c r="G56" t="n">
-        <v>62.423</v>
+        <v>40.07</v>
       </c>
       <c r="H56" t="n">
-        <v>59.675</v>
+        <v>40.31</v>
       </c>
       <c r="I56" t="n">
-        <v>57.896</v>
+        <v>39.86</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="C57" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="B57" s="1" t="n"/>
+      <c r="C57" s="1" t="n"/>
       <c r="D57" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>44.078</v>
+        <v>58.71</v>
       </c>
       <c r="F57" t="n">
-        <v>45.637</v>
+        <v>54.6</v>
       </c>
       <c r="G57" t="n">
-        <v>40.067</v>
+        <v>46.99</v>
       </c>
       <c r="H57" t="n">
-        <v>40.307</v>
+        <v>47.88</v>
       </c>
       <c r="I57" t="n">
-        <v>39.863</v>
+        <v>45.74</v>
       </c>
     </row>
     <row r="58">
@@ -2070,133 +2066,133 @@
       <c r="C58" s="1" t="n"/>
       <c r="D58" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>58.708</v>
+        <v>63.78</v>
       </c>
       <c r="F58" t="n">
-        <v>54.597</v>
+        <v>63.8</v>
       </c>
       <c r="G58" t="n">
-        <v>46.986</v>
+        <v>61.87</v>
       </c>
       <c r="H58" t="n">
-        <v>47.879</v>
+        <v>59.94</v>
       </c>
       <c r="I58" t="n">
-        <v>45.743</v>
+        <v>57.81</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n"/>
       <c r="B59" s="1" t="n"/>
-      <c r="C59" s="1" t="n"/>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D59" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>63.782</v>
+        <v>59.01</v>
       </c>
       <c r="F59" t="n">
-        <v>63.803</v>
+        <v>54.6</v>
       </c>
       <c r="G59" t="n">
-        <v>61.866</v>
+        <v>47.85</v>
       </c>
       <c r="H59" t="n">
-        <v>59.935</v>
+        <v>48.5</v>
       </c>
       <c r="I59" t="n">
-        <v>57.81</v>
+        <v>45.99</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
       <c r="B60" s="1" t="n"/>
-      <c r="C60" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C60" s="1" t="n"/>
       <c r="D60" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>59.011</v>
+        <v>64.17</v>
       </c>
       <c r="F60" t="n">
-        <v>54.605</v>
+        <v>64.41</v>
       </c>
       <c r="G60" t="n">
-        <v>47.849</v>
+        <v>62.94</v>
       </c>
       <c r="H60" t="n">
-        <v>48.504</v>
+        <v>60.4</v>
       </c>
       <c r="I60" t="n">
-        <v>45.991</v>
+        <v>57.76</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
-      <c r="B61" s="1" t="n"/>
-      <c r="C61" s="1" t="n"/>
+      <c r="B61" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D61" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>64.17</v>
+        <v>43.14</v>
       </c>
       <c r="F61" t="n">
-        <v>64.407</v>
+        <v>45.53</v>
       </c>
       <c r="G61" t="n">
-        <v>62.937</v>
+        <v>39.41</v>
       </c>
       <c r="H61" t="n">
-        <v>60.4</v>
+        <v>38.73</v>
       </c>
       <c r="I61" t="n">
-        <v>57.757</v>
+        <v>38.32</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n"/>
-      <c r="B62" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C62" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="B62" s="1" t="n"/>
+      <c r="C62" s="1" t="n"/>
       <c r="D62" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>43.142</v>
+        <v>58.46</v>
       </c>
       <c r="F62" t="n">
-        <v>45.528</v>
+        <v>53.4</v>
       </c>
       <c r="G62" t="n">
-        <v>39.406</v>
+        <v>46.5</v>
       </c>
       <c r="H62" t="n">
-        <v>38.726</v>
+        <v>47.2</v>
       </c>
       <c r="I62" t="n">
-        <v>38.322</v>
+        <v>44.94</v>
       </c>
     </row>
     <row r="63">
@@ -2205,133 +2201,133 @@
       <c r="C63" s="1" t="n"/>
       <c r="D63" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>58.458</v>
+        <v>63.66</v>
       </c>
       <c r="F63" t="n">
-        <v>53.402</v>
+        <v>63.63</v>
       </c>
       <c r="G63" t="n">
-        <v>46.497</v>
+        <v>62.02</v>
       </c>
       <c r="H63" t="n">
-        <v>47.202</v>
+        <v>59.96</v>
       </c>
       <c r="I63" t="n">
-        <v>44.943</v>
+        <v>57.94</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n"/>
       <c r="B64" s="1" t="n"/>
-      <c r="C64" s="1" t="n"/>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D64" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>63.659</v>
+        <v>58.81</v>
       </c>
       <c r="F64" t="n">
-        <v>63.629</v>
+        <v>53.7</v>
       </c>
       <c r="G64" t="n">
-        <v>62.022</v>
+        <v>47.19</v>
       </c>
       <c r="H64" t="n">
-        <v>59.965</v>
+        <v>48.22</v>
       </c>
       <c r="I64" t="n">
-        <v>57.944</v>
+        <v>45.19</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
       <c r="B65" s="1" t="n"/>
-      <c r="C65" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C65" s="1" t="n"/>
       <c r="D65" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>58.812</v>
+        <v>63.98</v>
       </c>
       <c r="F65" t="n">
-        <v>53.695</v>
+        <v>64.43000000000001</v>
       </c>
       <c r="G65" t="n">
-        <v>47.19</v>
+        <v>62.86</v>
       </c>
       <c r="H65" t="n">
-        <v>48.218</v>
+        <v>60.76</v>
       </c>
       <c r="I65" t="n">
-        <v>45.187</v>
+        <v>58.04</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
-      <c r="B66" s="1" t="n"/>
-      <c r="C66" s="1" t="n"/>
+      <c r="B66" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>bm25</t>
+        </is>
+      </c>
       <c r="D66" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>-----</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>63.976</v>
+        <v>42.9</v>
       </c>
       <c r="F66" t="n">
-        <v>64.43300000000001</v>
+        <v>45.43</v>
       </c>
       <c r="G66" t="n">
-        <v>62.864</v>
+        <v>39.42</v>
       </c>
       <c r="H66" t="n">
-        <v>60.758</v>
+        <v>38.42</v>
       </c>
       <c r="I66" t="n">
-        <v>58.039</v>
+        <v>37.95</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
-      <c r="B67" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="C67" s="1" t="inlineStr">
-        <is>
-          <t>bm25</t>
-        </is>
-      </c>
+      <c r="B67" s="1" t="n"/>
+      <c r="C67" s="1" t="n"/>
       <c r="D67" s="1" t="inlineStr">
         <is>
-          <t>-----</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>42.9</v>
+        <v>58.3</v>
       </c>
       <c r="F67" t="n">
-        <v>45.426</v>
+        <v>53.28</v>
       </c>
       <c r="G67" t="n">
-        <v>39.415</v>
+        <v>46.28</v>
       </c>
       <c r="H67" t="n">
-        <v>38.423</v>
+        <v>46.8</v>
       </c>
       <c r="I67" t="n">
-        <v>37.948</v>
+        <v>44.45</v>
       </c>
     </row>
     <row r="68">
@@ -2340,143 +2336,118 @@
       <c r="C68" s="1" t="n"/>
       <c r="D68" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>58.3</v>
+        <v>63.71</v>
       </c>
       <c r="F68" t="n">
-        <v>53.275</v>
+        <v>63.87</v>
       </c>
       <c r="G68" t="n">
-        <v>46.275</v>
+        <v>61.93</v>
       </c>
       <c r="H68" t="n">
-        <v>46.796</v>
+        <v>60</v>
       </c>
       <c r="I68" t="n">
-        <v>44.45</v>
+        <v>58.13</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
       <c r="B69" s="1" t="n"/>
-      <c r="C69" s="1" t="n"/>
+      <c r="C69" s="1" t="inlineStr">
+        <is>
+          <t>join</t>
+        </is>
+      </c>
       <c r="D69" s="1" t="inlineStr">
         <is>
-          <t>BASE</t>
+          <t>INDIR</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>63.711</v>
+        <v>58.61</v>
       </c>
       <c r="F69" t="n">
-        <v>63.873</v>
+        <v>53.68</v>
       </c>
       <c r="G69" t="n">
-        <v>61.929</v>
+        <v>47.09</v>
       </c>
       <c r="H69" t="n">
-        <v>60.004</v>
+        <v>47.64</v>
       </c>
       <c r="I69" t="n">
-        <v>58.128</v>
+        <v>44.82</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
       <c r="B70" s="1" t="n"/>
-      <c r="C70" s="1" t="inlineStr">
-        <is>
-          <t>join</t>
-        </is>
-      </c>
+      <c r="C70" s="1" t="n"/>
       <c r="D70" s="1" t="inlineStr">
         <is>
-          <t>INDIR</t>
+          <t>BASE</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>58.607</v>
+        <v>63.94</v>
       </c>
       <c r="F70" t="n">
-        <v>53.681</v>
+        <v>64.62</v>
       </c>
       <c r="G70" t="n">
-        <v>47.086</v>
+        <v>62.87</v>
       </c>
       <c r="H70" t="n">
-        <v>47.643</v>
+        <v>60.8</v>
       </c>
       <c r="I70" t="n">
-        <v>44.821</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n"/>
-      <c r="B71" s="1" t="n"/>
-      <c r="C71" s="1" t="n"/>
-      <c r="D71" s="1" t="inlineStr">
-        <is>
-          <t>BASE</t>
-        </is>
-      </c>
-      <c r="E71" t="n">
-        <v>63.945</v>
-      </c>
-      <c r="F71" t="n">
-        <v>64.623</v>
-      </c>
-      <c r="G71" t="n">
-        <v>62.869</v>
-      </c>
-      <c r="H71" t="n">
-        <v>60.803</v>
-      </c>
-      <c r="I71" t="n">
-        <v>58.336</v>
+        <v>58.34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="B26:B30"/>
     <mergeCell ref="E1:I1"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="A22:A71"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A12:A21"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B66:B70"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="A21:A70"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B21:B25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>